<commit_message>
Finalmente tudo funcionando Erro era que proximo teste e proxima recrga estavam com formulas nas celulas
</commit_message>
<xml_diff>
--- a/src/main/resources/extintores.xlsx
+++ b/src/main/resources/extintores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/534bce425fa7cd0e/Área de Trabalho/Extintor/EtiquetasExtintor/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{96D43180-B356-40E1-B4C4-9DBBC3644DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{298FFBF8-854A-4DB0-8221-38C0730BCBFC}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{96D43180-B356-40E1-B4C4-9DBBC3644DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66A5DA39-5DC1-4EA6-B1D3-8399F4882503}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{40751BAE-9F2C-437A-9AF3-44873B6C2F52}"/>
   </bookViews>
@@ -33,6 +33,43 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="2">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+  </valueMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1573,6 +1610,68 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>2</v>
+    <v>8</v>
+    <v>959</v>
+    <v>1</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_error">
+    <k n="colOffset" t="i"/>
+    <k n="errorType" t="i"/>
+    <k n="rwOffset" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+</rvStructures>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1894,8 +1993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30341ADD-E059-48DB-80AF-F3401B053938}">
   <dimension ref="A1:L582"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106:XFD106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1975,12 +2074,12 @@
         <v>11</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" ref="I3:I34" si="0">E3+375</f>
+        <f>E3+375</f>
         <v>46214</v>
       </c>
-      <c r="J3" s="1">
-        <f t="shared" ref="J3:J34" si="1">F3+5</f>
-        <v>2029</v>
+      <c r="J3" s="1" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="J3" ca="1">F3+A106:C1065</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2009,11 +2108,11 @@
         <v>10</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" si="0"/>
+        <f>E4+375</f>
         <v>46214</v>
       </c>
       <c r="J4" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J3:J34" si="0">F4+5</f>
         <v>2030</v>
       </c>
     </row>
@@ -2043,11 +2142,11 @@
         <v>9</v>
       </c>
       <c r="I5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I3:I34" si="1">E5+375</f>
         <v>46214</v>
       </c>
       <c r="J5" s="1">
-        <f t="shared" si="1"/>
+        <f>F5+5</f>
         <v>2030</v>
       </c>
     </row>
@@ -2077,11 +2176,11 @@
         <v>7</v>
       </c>
       <c r="I6" s="2">
+        <f t="shared" si="1"/>
+        <v>46002</v>
+      </c>
+      <c r="J6" s="1">
         <f t="shared" si="0"/>
-        <v>46002</v>
-      </c>
-      <c r="J6" s="1">
-        <f t="shared" si="1"/>
         <v>2029</v>
       </c>
     </row>
@@ -2111,11 +2210,11 @@
         <v>6</v>
       </c>
       <c r="I7" s="2">
+        <f t="shared" si="1"/>
+        <v>45849</v>
+      </c>
+      <c r="J7" s="1">
         <f t="shared" si="0"/>
-        <v>45849</v>
-      </c>
-      <c r="J7" s="1">
-        <f t="shared" si="1"/>
         <v>2025</v>
       </c>
     </row>
@@ -2145,11 +2244,11 @@
         <v>5</v>
       </c>
       <c r="I8" s="2">
+        <f t="shared" si="1"/>
+        <v>46214</v>
+      </c>
+      <c r="J8" s="1">
         <f t="shared" si="0"/>
-        <v>46214</v>
-      </c>
-      <c r="J8" s="1">
-        <f t="shared" si="1"/>
         <v>2028</v>
       </c>
       <c r="L8" s="26"/>
@@ -2180,11 +2279,11 @@
         <v>0</v>
       </c>
       <c r="I9" s="2">
+        <f t="shared" si="1"/>
+        <v>46002</v>
+      </c>
+      <c r="J9" s="1">
         <f t="shared" si="0"/>
-        <v>46002</v>
-      </c>
-      <c r="J9" s="1">
-        <f t="shared" si="1"/>
         <v>2029</v>
       </c>
     </row>
@@ -2214,11 +2313,11 @@
         <v>405</v>
       </c>
       <c r="I10" s="2">
+        <f t="shared" si="1"/>
+        <v>46214</v>
+      </c>
+      <c r="J10" s="1">
         <f t="shared" si="0"/>
-        <v>46214</v>
-      </c>
-      <c r="J10" s="1">
-        <f t="shared" si="1"/>
         <v>2026</v>
       </c>
     </row>
@@ -2248,11 +2347,11 @@
         <v>404</v>
       </c>
       <c r="I11" s="2">
+        <f t="shared" si="1"/>
+        <v>46214</v>
+      </c>
+      <c r="J11" s="1">
         <f t="shared" si="0"/>
-        <v>46214</v>
-      </c>
-      <c r="J11" s="1">
-        <f t="shared" si="1"/>
         <v>2030</v>
       </c>
     </row>
@@ -2282,11 +2381,11 @@
         <v>402</v>
       </c>
       <c r="I12" s="2">
+        <f t="shared" si="1"/>
+        <v>46002</v>
+      </c>
+      <c r="J12" s="1">
         <f t="shared" si="0"/>
-        <v>46002</v>
-      </c>
-      <c r="J12" s="1">
-        <f t="shared" si="1"/>
         <v>2029</v>
       </c>
     </row>
@@ -2316,11 +2415,11 @@
         <v>401</v>
       </c>
       <c r="I13" s="2">
+        <f t="shared" si="1"/>
+        <v>46214</v>
+      </c>
+      <c r="J13" s="1">
         <f t="shared" si="0"/>
-        <v>46214</v>
-      </c>
-      <c r="J13" s="1">
-        <f t="shared" si="1"/>
         <v>2030</v>
       </c>
     </row>
@@ -2350,11 +2449,11 @@
         <v>400</v>
       </c>
       <c r="I14" s="2">
+        <f t="shared" si="1"/>
+        <v>46214</v>
+      </c>
+      <c r="J14" s="1">
         <f t="shared" si="0"/>
-        <v>46214</v>
-      </c>
-      <c r="J14" s="1">
-        <f t="shared" si="1"/>
         <v>2028</v>
       </c>
     </row>
@@ -2384,11 +2483,11 @@
         <v>399</v>
       </c>
       <c r="I15" s="2">
+        <f t="shared" si="1"/>
+        <v>45790</v>
+      </c>
+      <c r="J15" s="1">
         <f t="shared" si="0"/>
-        <v>45790</v>
-      </c>
-      <c r="J15" s="1">
-        <f t="shared" si="1"/>
         <v>2029</v>
       </c>
     </row>
@@ -2418,11 +2517,11 @@
         <v>397</v>
       </c>
       <c r="I16" s="2">
+        <f t="shared" si="1"/>
+        <v>46002</v>
+      </c>
+      <c r="J16" s="1">
         <f t="shared" si="0"/>
-        <v>46002</v>
-      </c>
-      <c r="J16" s="1">
-        <f t="shared" si="1"/>
         <v>2029</v>
       </c>
     </row>
@@ -2452,11 +2551,11 @@
         <v>396</v>
       </c>
       <c r="I17" s="2">
+        <f t="shared" si="1"/>
+        <v>46214</v>
+      </c>
+      <c r="J17" s="1">
         <f t="shared" si="0"/>
-        <v>46214</v>
-      </c>
-      <c r="J17" s="1">
-        <f t="shared" si="1"/>
         <v>2028</v>
       </c>
     </row>
@@ -2486,11 +2585,11 @@
         <v>395</v>
       </c>
       <c r="I18" s="2">
+        <f t="shared" si="1"/>
+        <v>46214</v>
+      </c>
+      <c r="J18" s="1">
         <f t="shared" si="0"/>
-        <v>46214</v>
-      </c>
-      <c r="J18" s="1">
-        <f t="shared" si="1"/>
         <v>2029</v>
       </c>
     </row>
@@ -2520,11 +2619,11 @@
         <v>393</v>
       </c>
       <c r="I19" s="2">
+        <f t="shared" si="1"/>
+        <v>46002</v>
+      </c>
+      <c r="J19" s="1">
         <f t="shared" si="0"/>
-        <v>46002</v>
-      </c>
-      <c r="J19" s="1">
-        <f t="shared" si="1"/>
         <v>2029</v>
       </c>
     </row>
@@ -2554,11 +2653,11 @@
         <v>392</v>
       </c>
       <c r="I20" s="2">
+        <f t="shared" si="1"/>
+        <v>45849</v>
+      </c>
+      <c r="J20" s="1">
         <f t="shared" si="0"/>
-        <v>45849</v>
-      </c>
-      <c r="J20" s="1">
-        <f t="shared" si="1"/>
         <v>2026</v>
       </c>
     </row>
@@ -2588,11 +2687,11 @@
         <v>390</v>
       </c>
       <c r="I21" s="2">
+        <f t="shared" si="1"/>
+        <v>46002</v>
+      </c>
+      <c r="J21" s="1">
         <f t="shared" si="0"/>
-        <v>46002</v>
-      </c>
-      <c r="J21" s="1">
-        <f t="shared" si="1"/>
         <v>2029</v>
       </c>
     </row>
@@ -2622,11 +2721,11 @@
         <v>389</v>
       </c>
       <c r="I22" s="2">
+        <f t="shared" si="1"/>
+        <v>45972</v>
+      </c>
+      <c r="J22" s="1">
         <f t="shared" si="0"/>
-        <v>45972</v>
-      </c>
-      <c r="J22" s="1">
-        <f t="shared" si="1"/>
         <v>2026</v>
       </c>
     </row>
@@ -2656,11 +2755,11 @@
         <v>388</v>
       </c>
       <c r="I23" s="2">
+        <f t="shared" si="1"/>
+        <v>45941</v>
+      </c>
+      <c r="J23" s="24">
         <f t="shared" si="0"/>
-        <v>45941</v>
-      </c>
-      <c r="J23" s="24">
-        <f t="shared" si="1"/>
         <v>2028</v>
       </c>
     </row>
@@ -2690,11 +2789,11 @@
         <v>387</v>
       </c>
       <c r="I24" s="2">
+        <f t="shared" si="1"/>
+        <v>45972</v>
+      </c>
+      <c r="J24" s="1">
         <f t="shared" si="0"/>
-        <v>45972</v>
-      </c>
-      <c r="J24" s="1">
-        <f t="shared" si="1"/>
         <v>2028</v>
       </c>
     </row>
@@ -2724,11 +2823,11 @@
         <v>386</v>
       </c>
       <c r="I25" s="2">
+        <f t="shared" si="1"/>
+        <v>45972</v>
+      </c>
+      <c r="J25" s="1">
         <f t="shared" si="0"/>
-        <v>45972</v>
-      </c>
-      <c r="J25" s="1">
-        <f t="shared" si="1"/>
         <v>2025</v>
       </c>
     </row>
@@ -2758,11 +2857,11 @@
         <v>385</v>
       </c>
       <c r="I26" s="2">
+        <f t="shared" si="1"/>
+        <v>46214</v>
+      </c>
+      <c r="J26" s="1">
         <f t="shared" si="0"/>
-        <v>46214</v>
-      </c>
-      <c r="J26" s="1">
-        <f t="shared" si="1"/>
         <v>2030</v>
       </c>
     </row>
@@ -2792,11 +2891,11 @@
         <v>384</v>
       </c>
       <c r="I27" s="2">
+        <f t="shared" si="1"/>
+        <v>45788</v>
+      </c>
+      <c r="J27" s="1">
         <f t="shared" si="0"/>
-        <v>45788</v>
-      </c>
-      <c r="J27" s="1">
-        <f t="shared" si="1"/>
         <v>2026</v>
       </c>
     </row>
@@ -2826,11 +2925,11 @@
         <v>383</v>
       </c>
       <c r="I28" s="2">
+        <f t="shared" si="1"/>
+        <v>45972</v>
+      </c>
+      <c r="J28" s="1">
         <f t="shared" si="0"/>
-        <v>45972</v>
-      </c>
-      <c r="J28" s="1">
-        <f t="shared" si="1"/>
         <v>2025</v>
       </c>
     </row>
@@ -2860,11 +2959,11 @@
         <v>382</v>
       </c>
       <c r="I29" s="2">
+        <f t="shared" si="1"/>
+        <v>45972</v>
+      </c>
+      <c r="J29" s="1">
         <f t="shared" si="0"/>
-        <v>45972</v>
-      </c>
-      <c r="J29" s="1">
-        <f t="shared" si="1"/>
         <v>2025</v>
       </c>
     </row>
@@ -2894,11 +2993,11 @@
         <v>381</v>
       </c>
       <c r="I30" s="2">
+        <f t="shared" si="1"/>
+        <v>45941</v>
+      </c>
+      <c r="J30" s="1">
         <f t="shared" si="0"/>
-        <v>45941</v>
-      </c>
-      <c r="J30" s="1">
-        <f t="shared" si="1"/>
         <v>2028</v>
       </c>
     </row>
@@ -2928,11 +3027,11 @@
         <v>380</v>
       </c>
       <c r="I31" s="2">
+        <f t="shared" si="1"/>
+        <v>45667</v>
+      </c>
+      <c r="J31" s="1">
         <f t="shared" si="0"/>
-        <v>45667</v>
-      </c>
-      <c r="J31" s="1">
-        <f t="shared" si="1"/>
         <v>2025</v>
       </c>
     </row>
@@ -2962,11 +3061,11 @@
         <v>379</v>
       </c>
       <c r="I32" s="2">
+        <f t="shared" si="1"/>
+        <v>45941</v>
+      </c>
+      <c r="J32" s="1">
         <f t="shared" si="0"/>
-        <v>45941</v>
-      </c>
-      <c r="J32" s="1">
-        <f t="shared" si="1"/>
         <v>2028</v>
       </c>
     </row>
@@ -2996,11 +3095,11 @@
         <v>378</v>
       </c>
       <c r="I33" s="2">
+        <f t="shared" si="1"/>
+        <v>45819</v>
+      </c>
+      <c r="J33" s="1">
         <f t="shared" si="0"/>
-        <v>45819</v>
-      </c>
-      <c r="J33" s="1">
-        <f t="shared" si="1"/>
         <v>2027</v>
       </c>
     </row>
@@ -3030,11 +3129,11 @@
         <v>377</v>
       </c>
       <c r="I34" s="2">
+        <f t="shared" si="1"/>
+        <v>45788</v>
+      </c>
+      <c r="J34" s="1">
         <f t="shared" si="0"/>
-        <v>45788</v>
-      </c>
-      <c r="J34" s="1">
-        <f t="shared" si="1"/>
         <v>2025</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Falta definir o nome da impressora em InterfaceExtintor e testar
</commit_message>
<xml_diff>
--- a/src/main/resources/extintores.xlsx
+++ b/src/main/resources/extintores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/534bce425fa7cd0e/Área de Trabalho/Extintor/EtiquetasExtintor/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{96D43180-B356-40E1-B4C4-9DBBC3644DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66A5DA39-5DC1-4EA6-B1D3-8399F4882503}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{96D43180-B356-40E1-B4C4-9DBBC3644DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60BE6E4C-B43B-4AA3-9ED7-2AB5DF47EB78}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{40751BAE-9F2C-437A-9AF3-44873B6C2F52}"/>
   </bookViews>
@@ -33,43 +33,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="2">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <futureMetadata name="XLRICHVALUE" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-  <valueMetadata count="1">
-    <bk>
-      <rc t="2" v="0"/>
-    </bk>
-  </valueMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1610,68 +1573,6 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <global>
-    <keyFlags>
-      <key name="_Self">
-        <flag name="ExcludeFromFile" value="1"/>
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_DisplayString">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Flags">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Format">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_SubLabel">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Attribution">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Icon">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Display">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_CanonicalPropertyNames">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_ClassificationId">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-    </keyFlags>
-  </global>
-</rvTypesInfo>
-</file>
-
-<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <rv s="0">
-    <v>2</v>
-    <v>8</v>
-    <v>959</v>
-    <v>1</v>
-  </rv>
-</rvData>
-</file>
-
-<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <s t="_error">
-    <k n="colOffset" t="i"/>
-    <k n="errorType" t="i"/>
-    <k n="rwOffset" t="i"/>
-    <k n="subType" t="i"/>
-  </s>
-</rvStructures>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1993,8 +1894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30341ADD-E059-48DB-80AF-F3401B053938}">
   <dimension ref="A1:L582"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A106" sqref="A106:XFD106"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2077,9 +1978,9 @@
         <f>E3+375</f>
         <v>46214</v>
       </c>
-      <c r="J3" s="1" t="e" cm="1" vm="1">
-        <f t="array" aca="1" ref="J3" ca="1">F3+A106:C1065</f>
-        <v>#VALUE!</v>
+      <c r="J3" s="10">
+        <f>F3+5</f>
+        <v>2029</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2112,7 +2013,7 @@
         <v>46214</v>
       </c>
       <c r="J4" s="10">
-        <f t="shared" ref="J3:J34" si="0">F4+5</f>
+        <f t="shared" ref="J4:J34" si="0">F4+5</f>
         <v>2030</v>
       </c>
     </row>
@@ -2142,7 +2043,7 @@
         <v>9</v>
       </c>
       <c r="I5" s="2">
-        <f t="shared" ref="I3:I34" si="1">E5+375</f>
+        <f t="shared" ref="I5:I34" si="1">E5+375</f>
         <v>46214</v>
       </c>
       <c r="J5" s="1">

</xml_diff>